<commit_message>
18.12.2023, Tasterfunktion + Projektdokumentation geupdatet
</commit_message>
<xml_diff>
--- a/Project_Car_01_Documentation.xlsx
+++ b/Project_Car_01_Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\group-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FC3390-39DF-4C39-9C20-A41CF647C9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3C4E4D-62D3-4CA1-B535-B6F51D246F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="237">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1153,6 +1153,12 @@
   </si>
   <si>
     <t>Fehlersuche beim Motorshield, Wackelkontakte bei den Motoren verzinnt und in Betrieb genommen</t>
+  </si>
+  <si>
+    <t>Start und Stoptaster programmiert</t>
+  </si>
+  <si>
+    <t>Erkennung von Anfang der Kurve mittels des mittleren Infrarotsensor</t>
   </si>
 </sst>
 </file>
@@ -1861,6 +1867,33 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1879,33 +1912,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1929,9 +1938,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2418,14 +2424,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="110" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -2474,10 +2480,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="115" t="s">
+      <c r="E7" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="115"/>
+      <c r="F7" s="111"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -2488,8 +2494,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="121"/>
-      <c r="F8" s="121"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2500,8 +2506,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="122"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
@@ -2512,8 +2518,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="123"/>
-      <c r="F10" s="123"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2524,8 +2530,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="117"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="115"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="17"/>
@@ -2546,49 +2552,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="118"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="116"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="119"/>
-      <c r="C16" s="119"/>
-      <c r="D16" s="119"/>
-      <c r="E16" s="119"/>
-      <c r="F16" s="119"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="117"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="119"/>
-      <c r="C17" s="119"/>
-      <c r="D17" s="119"/>
-      <c r="E17" s="119"/>
-      <c r="F17" s="119"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="119"/>
-      <c r="C18" s="119"/>
-      <c r="D18" s="119"/>
-      <c r="E18" s="119"/>
-      <c r="F18" s="119"/>
+      <c r="B18" s="117"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="113"/>
-      <c r="C19" s="113"/>
-      <c r="D19" s="113"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="113"/>
+      <c r="B19" s="122"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="122"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="122"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
@@ -2601,74 +2607,64 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="114" t="s">
+      <c r="A23" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="114"/>
-      <c r="C23" s="114"/>
-      <c r="D23" s="114"/>
-      <c r="E23" s="114"/>
-      <c r="F23" s="114"/>
+      <c r="B23" s="123"/>
+      <c r="C23" s="123"/>
+      <c r="D23" s="123"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="123"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="115" t="s">
+      <c r="A26" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="115"/>
-      <c r="C26" s="115"/>
-      <c r="D26" s="115" t="s">
+      <c r="B26" s="111"/>
+      <c r="C26" s="111"/>
+      <c r="D26" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="115"/>
-      <c r="F26" s="115"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="111"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="110" t="s">
+      <c r="A27" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="110"/>
-      <c r="C27" s="110"/>
-      <c r="D27" s="116"/>
-      <c r="E27" s="116"/>
-      <c r="F27" s="116"/>
+      <c r="B27" s="119"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="124"/>
+      <c r="E27" s="124"/>
+      <c r="F27" s="124"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="109" t="s">
+      <c r="A28" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="109"/>
-      <c r="C28" s="109"/>
-      <c r="D28" s="110" t="s">
+      <c r="B28" s="118"/>
+      <c r="C28" s="118"/>
+      <c r="D28" s="119" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="110"/>
-      <c r="F28" s="110"/>
+      <c r="E28" s="119"/>
+      <c r="F28" s="119"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="111" t="s">
+      <c r="A29" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="111"/>
-      <c r="C29" s="111"/>
-      <c r="D29" s="112"/>
-      <c r="E29" s="112"/>
-      <c r="F29" s="112"/>
+      <c r="B29" s="120"/>
+      <c r="C29" s="120"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="121"/>
+      <c r="F29" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2679,6 +2675,16 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2690,8 +2696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E282F0E-D68B-4ABC-BD94-0D22FA301A66}">
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2703,11 +2709,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="126" t="s">
         <v>218</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
     </row>
     <row r="3" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
@@ -2831,7 +2837,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="132">
+      <c r="A14" s="109">
         <v>45271</v>
       </c>
       <c r="B14" s="41">
@@ -2842,14 +2848,26 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="40">
+        <v>45278</v>
+      </c>
+      <c r="B15" s="41">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="40">
+        <v>45278</v>
+      </c>
+      <c r="B16" s="41">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="41"/>
@@ -3010,29 +3028,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="125" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="124"/>
+      <c r="C3" s="125"/>
     </row>
     <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="125" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="124"/>
+      <c r="C4" s="125"/>
     </row>
     <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="125" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="124"/>
+      <c r="C5" s="125"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
@@ -3255,11 +3273,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="126" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="35"/>
@@ -3267,18 +3285,18 @@
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="126" t="s">
+      <c r="A3" s="127" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="127"/>
     </row>
     <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="127"/>
-      <c r="C4" s="127"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="128"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="35"/>
@@ -3558,14 +3576,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="126" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
     </row>
     <row r="3" spans="1:6" s="43" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -3858,16 +3876,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
     </row>
     <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -4508,19 +4526,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="129" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="129"/>
     </row>
     <row r="3" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="74" t="s">
@@ -5184,16 +5202,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="126" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E2" s="36"/>
@@ -5969,71 +5987,71 @@
       <c r="A21" s="97" t="s">
         <v>160</v>
       </c>
-      <c r="B21" s="130" t="s">
+      <c r="B21" s="131" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="130"/>
-      <c r="D21" s="130"/>
+      <c r="C21" s="131"/>
+      <c r="D21" s="131"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="102" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="131" t="s">
+      <c r="B22" s="132" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="131"/>
-      <c r="D22" s="131"/>
+      <c r="C22" s="132"/>
+      <c r="D22" s="132"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="102" t="s">
         <v>190</v>
       </c>
-      <c r="B23" s="131" t="s">
+      <c r="B23" s="132" t="s">
         <v>191</v>
       </c>
-      <c r="C23" s="131"/>
-      <c r="D23" s="131"/>
+      <c r="C23" s="132"/>
+      <c r="D23" s="132"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="102" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="131" t="s">
+      <c r="B24" s="132" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="131"/>
-      <c r="D24" s="131"/>
+      <c r="C24" s="132"/>
+      <c r="D24" s="132"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="99"/>
-      <c r="B25" s="129"/>
-      <c r="C25" s="129"/>
-      <c r="D25" s="129"/>
+      <c r="B25" s="130"/>
+      <c r="C25" s="130"/>
+      <c r="D25" s="130"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="99"/>
-      <c r="B26" s="129"/>
-      <c r="C26" s="129"/>
-      <c r="D26" s="129"/>
+      <c r="B26" s="130"/>
+      <c r="C26" s="130"/>
+      <c r="D26" s="130"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="99"/>
-      <c r="B27" s="129"/>
-      <c r="C27" s="129"/>
-      <c r="D27" s="129"/>
+      <c r="B27" s="130"/>
+      <c r="C27" s="130"/>
+      <c r="D27" s="130"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="99"/>
-      <c r="B28" s="129"/>
-      <c r="C28" s="129"/>
-      <c r="D28" s="129"/>
+      <c r="B28" s="130"/>
+      <c r="C28" s="130"/>
+      <c r="D28" s="130"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="99"/>
-      <c r="B29" s="129"/>
-      <c r="C29" s="129"/>
-      <c r="D29" s="129"/>
+      <c r="B29" s="130"/>
+      <c r="C29" s="130"/>
+      <c r="D29" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -6070,8 +6088,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6083,11 +6101,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="126" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
     </row>
     <row r="3" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -6244,14 +6262,26 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="40">
+        <v>45278</v>
+      </c>
+      <c r="B17" s="41">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="40">
+        <v>45278</v>
+      </c>
+      <c r="B18" s="41">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="41"/>

</xml_diff>

<commit_message>
Code editiert und Dokumentation
</commit_message>
<xml_diff>
--- a/Project_Car_01_Documentation.xlsx
+++ b/Project_Car_01_Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\group-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3C4E4D-62D3-4CA1-B535-B6F51D246F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79453F92-2F5F-4802-A764-3D3344F5FCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="240">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1159,6 +1159,15 @@
   </si>
   <si>
     <t>Erkennung von Anfang der Kurve mittels des mittleren Infrarotsensor</t>
+  </si>
+  <si>
+    <t>Fehlerbehebung (Motorenverbindungen, Akkuhalterung austauschen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State-Machine skizzieren </t>
+  </si>
+  <si>
+    <t>Fehlersuche für gepfuschte Hardware und Software</t>
   </si>
 </sst>
 </file>
@@ -1870,12 +1879,42 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1884,36 +1923,6 @@
     </xf>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2424,14 +2433,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -2480,10 +2489,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="111" t="s">
+      <c r="E7" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="111"/>
+      <c r="F7" s="116"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -2494,8 +2503,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2506,8 +2515,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="113"/>
-      <c r="F9" s="113"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
@@ -2518,8 +2527,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="114"/>
-      <c r="F10" s="114"/>
+      <c r="E10" s="124"/>
+      <c r="F10" s="124"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2530,8 +2539,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="17"/>
@@ -2552,49 +2561,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="116"/>
-      <c r="C15" s="116"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
-      <c r="F15" s="116"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="117"/>
-      <c r="C17" s="117"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="120"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="117"/>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
+      <c r="B18" s="120"/>
+      <c r="C18" s="120"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="122"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="122"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="114"/>
+      <c r="D19" s="114"/>
+      <c r="E19" s="114"/>
+      <c r="F19" s="114"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
@@ -2607,64 +2616,74 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="123" t="s">
+      <c r="A23" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
+      <c r="B23" s="115"/>
+      <c r="C23" s="115"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="115"/>
+      <c r="F23" s="115"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="111" t="s">
+      <c r="A26" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="111"/>
-      <c r="C26" s="111"/>
-      <c r="D26" s="111" t="s">
+      <c r="B26" s="116"/>
+      <c r="C26" s="116"/>
+      <c r="D26" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
+      <c r="E26" s="116"/>
+      <c r="F26" s="116"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="119" t="s">
+      <c r="A27" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="119"/>
-      <c r="C27" s="119"/>
-      <c r="D27" s="124"/>
-      <c r="E27" s="124"/>
-      <c r="F27" s="124"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="118" t="s">
+      <c r="A28" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="118"/>
-      <c r="C28" s="118"/>
-      <c r="D28" s="119" t="s">
+      <c r="B28" s="110"/>
+      <c r="C28" s="110"/>
+      <c r="D28" s="111" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="111"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="120" t="s">
+      <c r="A29" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="120"/>
-      <c r="C29" s="120"/>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="121"/>
+      <c r="B29" s="112"/>
+      <c r="C29" s="112"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="113"/>
+      <c r="F29" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2675,16 +2694,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2697,7 +2706,7 @@
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2870,14 +2879,26 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="40">
+        <v>45299</v>
+      </c>
+      <c r="B17" s="41">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="40">
+        <v>45299</v>
+      </c>
+      <c r="B18" s="41">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="41"/>
@@ -3028,11 +3049,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="125" t="s">
@@ -3876,16 +3897,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
     </row>
     <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -6089,7 +6110,7 @@
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A20" sqref="A20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6284,14 +6305,26 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="40">
+        <v>45299</v>
+      </c>
+      <c r="B19" s="41">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="40">
+        <v>45299</v>
+      </c>
+      <c r="B20" s="41">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="41"/>

</xml_diff>

<commit_message>
22.01.2024, Code und AZE aktualisiert
</commit_message>
<xml_diff>
--- a/Project_Car_01_Documentation.xlsx
+++ b/Project_Car_01_Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\group-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5427C9DA-F902-408A-9EE2-B6C71F7B220F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C0BE2A-0538-48AC-84A7-F66089A95A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8964" tabRatio="500" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="242">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1171,6 +1171,9 @@
   </si>
   <si>
     <t>Sate-Machine in Code implementieren</t>
+  </si>
+  <si>
+    <t>Feinjustierung der Threshholdwerte</t>
   </si>
 </sst>
 </file>
@@ -1882,12 +1885,42 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1896,36 +1929,6 @@
     </xf>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2436,14 +2439,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -2492,10 +2495,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="111" t="s">
+      <c r="E7" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="111"/>
+      <c r="F7" s="116"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -2506,8 +2509,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2518,8 +2521,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="113"/>
-      <c r="F9" s="113"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
@@ -2530,8 +2533,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="114"/>
-      <c r="F10" s="114"/>
+      <c r="E10" s="124"/>
+      <c r="F10" s="124"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2542,8 +2545,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="17"/>
@@ -2564,49 +2567,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="116"/>
-      <c r="C15" s="116"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
-      <c r="F15" s="116"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="117"/>
-      <c r="C17" s="117"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="120"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="117"/>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
+      <c r="B18" s="120"/>
+      <c r="C18" s="120"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="122"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="122"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="114"/>
+      <c r="D19" s="114"/>
+      <c r="E19" s="114"/>
+      <c r="F19" s="114"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
@@ -2619,64 +2622,74 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="123" t="s">
+      <c r="A23" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
+      <c r="B23" s="115"/>
+      <c r="C23" s="115"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="115"/>
+      <c r="F23" s="115"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="111" t="s">
+      <c r="A26" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="111"/>
-      <c r="C26" s="111"/>
-      <c r="D26" s="111" t="s">
+      <c r="B26" s="116"/>
+      <c r="C26" s="116"/>
+      <c r="D26" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
+      <c r="E26" s="116"/>
+      <c r="F26" s="116"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="119" t="s">
+      <c r="A27" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="119"/>
-      <c r="C27" s="119"/>
-      <c r="D27" s="124"/>
-      <c r="E27" s="124"/>
-      <c r="F27" s="124"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="118" t="s">
+      <c r="A28" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="118"/>
-      <c r="C28" s="118"/>
-      <c r="D28" s="119" t="s">
+      <c r="B28" s="110"/>
+      <c r="C28" s="110"/>
+      <c r="D28" s="111" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="111"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="120" t="s">
+      <c r="A29" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="120"/>
-      <c r="C29" s="120"/>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="121"/>
+      <c r="B29" s="112"/>
+      <c r="C29" s="112"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="113"/>
+      <c r="F29" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2687,16 +2700,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2708,8 +2711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E282F0E-D68B-4ABC-BD94-0D22FA301A66}">
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2915,9 +2918,15 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="40">
+        <v>45313</v>
+      </c>
+      <c r="B20" s="41">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="41"/>
@@ -3058,11 +3067,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="125" t="s">
@@ -3906,16 +3915,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
     </row>
     <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -4220,7 +4229,7 @@
       </c>
       <c r="I17" s="59"/>
     </row>
-    <row r="18" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
         <v>32</v>
       </c>
@@ -6122,8 +6131,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="A22:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6351,9 +6360,15 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="40">
+        <v>45313</v>
+      </c>
+      <c r="B22" s="41">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="41"/>

</xml_diff>

<commit_message>
neuer Code mit Ringbuffer 🕳, Doc. aktualisiert
</commit_message>
<xml_diff>
--- a/Project_Car_01_Documentation.xlsx
+++ b/Project_Car_01_Documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\group-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C0BE2A-0538-48AC-84A7-F66089A95A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A0DC79-CFE2-4E1D-A4D4-2C17CE17B4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8964" tabRatio="500" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="243">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1174,6 +1174,9 @@
   </si>
   <si>
     <t>Feinjustierung der Threshholdwerte</t>
+  </si>
+  <si>
+    <t>Sensor neugelötet, um Messschwankungen bei der Messung zu minimieren, Ringpuffer für Sensorwerte implementiert</t>
   </si>
 </sst>
 </file>
@@ -1885,6 +1888,30 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1903,32 +1930,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2439,14 +2442,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="110" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -2495,10 +2498,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="116" t="s">
+      <c r="E7" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="116"/>
+      <c r="F7" s="111"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -2509,8 +2512,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="122"/>
-      <c r="F8" s="122"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2521,8 +2524,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
@@ -2533,8 +2536,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="124"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2545,8 +2548,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="115"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="17"/>
@@ -2567,49 +2570,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="119"/>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="119"/>
-      <c r="F15" s="119"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="116"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="120"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="117"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="120"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="120"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="120"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
+      <c r="B18" s="117"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="114"/>
-      <c r="C19" s="114"/>
-      <c r="D19" s="114"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="114"/>
+      <c r="B19" s="122"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="122"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="122"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
@@ -2622,74 +2625,64 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="115" t="s">
+      <c r="A23" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="115"/>
-      <c r="C23" s="115"/>
-      <c r="D23" s="115"/>
-      <c r="E23" s="115"/>
-      <c r="F23" s="115"/>
+      <c r="B23" s="123"/>
+      <c r="C23" s="123"/>
+      <c r="D23" s="123"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="123"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="116" t="s">
+      <c r="A26" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="116"/>
-      <c r="C26" s="116"/>
-      <c r="D26" s="116" t="s">
+      <c r="B26" s="111"/>
+      <c r="C26" s="111"/>
+      <c r="D26" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="116"/>
-      <c r="F26" s="116"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="111"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="111" t="s">
+      <c r="A27" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="111"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="117"/>
-      <c r="E27" s="117"/>
-      <c r="F27" s="117"/>
+      <c r="B27" s="119"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="124"/>
+      <c r="E27" s="124"/>
+      <c r="F27" s="124"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="110" t="s">
+      <c r="A28" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="110"/>
-      <c r="C28" s="110"/>
-      <c r="D28" s="111" t="s">
+      <c r="B28" s="118"/>
+      <c r="C28" s="118"/>
+      <c r="D28" s="119" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="111"/>
-      <c r="F28" s="111"/>
+      <c r="E28" s="119"/>
+      <c r="F28" s="119"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="112" t="s">
+      <c r="A29" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="112"/>
-      <c r="C29" s="112"/>
-      <c r="D29" s="113"/>
-      <c r="E29" s="113"/>
-      <c r="F29" s="113"/>
+      <c r="B29" s="120"/>
+      <c r="C29" s="120"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="121"/>
+      <c r="F29" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2700,6 +2693,16 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2711,8 +2714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E282F0E-D68B-4ABC-BD94-0D22FA301A66}">
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2928,10 +2931,16 @@
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="2"/>
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="40">
+        <v>45334</v>
+      </c>
+      <c r="B21" s="41">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="41"/>
@@ -3005,7 +3014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -3053,7 +3062,7 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -3067,11 +3076,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="125" t="s">
@@ -3301,7 +3310,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3599,7 +3608,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ21"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -3915,16 +3924,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
     </row>
     <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -6131,8 +6140,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="A22:C22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6370,10 +6379,16 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="41"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="2"/>
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="40">
+        <v>45334</v>
+      </c>
+      <c r="B23" s="41">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="41"/>

</xml_diff>

<commit_message>
AZE aktualisiert, Code umgeschrieben
</commit_message>
<xml_diff>
--- a/Project_Car_01_Documentation.xlsx
+++ b/Project_Car_01_Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\group-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A0DC79-CFE2-4E1D-A4D4-2C17CE17B4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4627576-F1CA-47F4-A834-DA02E4CC5B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="245">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1177,6 +1177,12 @@
   </si>
   <si>
     <t>Sensor neugelötet, um Messschwankungen bei der Messung zu minimieren, Ringpuffer für Sensorwerte implementiert</t>
+  </si>
+  <si>
+    <t>Besprechung über Implementierung von PID-Regler</t>
+  </si>
+  <si>
+    <t>Code optimieren</t>
   </si>
 </sst>
 </file>
@@ -1888,12 +1894,42 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1902,36 +1938,6 @@
     </xf>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2427,8 +2433,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J17" activeCellId="1" sqref="E13 J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2442,14 +2448,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -2498,10 +2504,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="111" t="s">
+      <c r="E7" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="111"/>
+      <c r="F7" s="116"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -2512,8 +2518,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2524,8 +2530,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="113"/>
-      <c r="F9" s="113"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
@@ -2536,8 +2542,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="114"/>
-      <c r="F10" s="114"/>
+      <c r="E10" s="124"/>
+      <c r="F10" s="124"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2548,8 +2554,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="17"/>
@@ -2570,49 +2576,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="116"/>
-      <c r="C15" s="116"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
-      <c r="F15" s="116"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="117"/>
-      <c r="C17" s="117"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="120"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="117"/>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
+      <c r="B18" s="120"/>
+      <c r="C18" s="120"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="122"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="122"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="114"/>
+      <c r="D19" s="114"/>
+      <c r="E19" s="114"/>
+      <c r="F19" s="114"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
@@ -2625,64 +2631,74 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="123" t="s">
+      <c r="A23" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
+      <c r="B23" s="115"/>
+      <c r="C23" s="115"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="115"/>
+      <c r="F23" s="115"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="111" t="s">
+      <c r="A26" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="111"/>
-      <c r="C26" s="111"/>
-      <c r="D26" s="111" t="s">
+      <c r="B26" s="116"/>
+      <c r="C26" s="116"/>
+      <c r="D26" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
+      <c r="E26" s="116"/>
+      <c r="F26" s="116"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="119" t="s">
+      <c r="A27" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="119"/>
-      <c r="C27" s="119"/>
-      <c r="D27" s="124"/>
-      <c r="E27" s="124"/>
-      <c r="F27" s="124"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="118" t="s">
+      <c r="A28" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="118"/>
-      <c r="C28" s="118"/>
-      <c r="D28" s="119" t="s">
+      <c r="B28" s="110"/>
+      <c r="C28" s="110"/>
+      <c r="D28" s="111" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="111"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="120" t="s">
+      <c r="A29" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="120"/>
-      <c r="C29" s="120"/>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="121"/>
+      <c r="B29" s="112"/>
+      <c r="C29" s="112"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="113"/>
+      <c r="F29" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2693,16 +2709,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2715,7 +2721,7 @@
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2943,14 +2949,26 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="40">
+        <v>45348</v>
+      </c>
+      <c r="B22" s="41">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="41"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="40">
+        <v>45348</v>
+      </c>
+      <c r="B23" s="41">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="41"/>
@@ -3062,7 +3080,7 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -3076,11 +3094,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="125" t="s">
@@ -3924,16 +3942,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
     </row>
     <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -6140,8 +6158,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="A25:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6391,14 +6409,26 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="2"/>
+      <c r="A24" s="40">
+        <v>45348</v>
+      </c>
+      <c r="B24" s="41">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="2"/>
+      <c r="A25" s="40">
+        <v>45348</v>
+      </c>
+      <c r="B25" s="41">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="41"/>

</xml_diff>

<commit_message>
PSP aktualisiert (Datum, Kommentar, Stunden)
</commit_message>
<xml_diff>
--- a/Project_Car_01_Documentation.xlsx
+++ b/Project_Car_01_Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\group-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4627576-F1CA-47F4-A834-DA02E4CC5B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293FD148-8AD8-4BC3-AA52-14E91C4D2989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="254">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1182,7 +1182,34 @@
     <t>Besprechung über Implementierung von PID-Regler</t>
   </si>
   <si>
-    <t>Code optimieren</t>
+    <t>Fahrzeug-Chassis wurde fertig übergeben</t>
+  </si>
+  <si>
+    <t>0,5 Stunden für die erste Inbetriebnahme, die restlichen kommen von Reparaturen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drive-Funktion Implementiert </t>
+  </si>
+  <si>
+    <t>Stoptaster als Interrupt, und Starttaster normal</t>
+  </si>
+  <si>
+    <t>3x Sharp Infrarotsensoren</t>
+  </si>
+  <si>
+    <t>2h für die Verlötung der Verbindungen, 2h für das genaue mitteln der Sensorwerte</t>
+  </si>
+  <si>
+    <t>mit gemittelten Werten</t>
+  </si>
+  <si>
+    <t>mittels Interrupt</t>
+  </si>
+  <si>
+    <t>nicht geplant</t>
+  </si>
+  <si>
+    <t>Programmcode optimiert</t>
   </si>
 </sst>
 </file>
@@ -1894,6 +1921,30 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1912,32 +1963,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2132,9 +2159,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2172,7 +2199,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2278,7 +2305,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2420,7 +2447,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2433,8 +2460,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J17" activeCellId="1" sqref="E13 J17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2448,14 +2475,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="110" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -2504,10 +2531,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="116" t="s">
+      <c r="E7" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="116"/>
+      <c r="F7" s="111"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -2518,8 +2545,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="122"/>
-      <c r="F8" s="122"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2530,8 +2557,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
@@ -2542,8 +2569,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="124"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2554,8 +2581,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="115"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="17"/>
@@ -2576,49 +2603,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="119"/>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="119"/>
-      <c r="F15" s="119"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="116"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="120"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="117"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="120"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="120"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="120"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
+      <c r="B18" s="117"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="114"/>
-      <c r="C19" s="114"/>
-      <c r="D19" s="114"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="114"/>
+      <c r="B19" s="122"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="122"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="122"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
@@ -2631,74 +2658,64 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="115" t="s">
+      <c r="A23" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="115"/>
-      <c r="C23" s="115"/>
-      <c r="D23" s="115"/>
-      <c r="E23" s="115"/>
-      <c r="F23" s="115"/>
+      <c r="B23" s="123"/>
+      <c r="C23" s="123"/>
+      <c r="D23" s="123"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="123"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="116" t="s">
+      <c r="A26" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="116"/>
-      <c r="C26" s="116"/>
-      <c r="D26" s="116" t="s">
+      <c r="B26" s="111"/>
+      <c r="C26" s="111"/>
+      <c r="D26" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="116"/>
-      <c r="F26" s="116"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="111"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="111" t="s">
+      <c r="A27" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="111"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="117"/>
-      <c r="E27" s="117"/>
-      <c r="F27" s="117"/>
+      <c r="B27" s="119"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="124"/>
+      <c r="E27" s="124"/>
+      <c r="F27" s="124"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="110" t="s">
+      <c r="A28" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="110"/>
-      <c r="C28" s="110"/>
-      <c r="D28" s="111" t="s">
+      <c r="B28" s="118"/>
+      <c r="C28" s="118"/>
+      <c r="D28" s="119" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="111"/>
-      <c r="F28" s="111"/>
+      <c r="E28" s="119"/>
+      <c r="F28" s="119"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="112" t="s">
+      <c r="A29" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="112"/>
-      <c r="C29" s="112"/>
-      <c r="D29" s="113"/>
-      <c r="E29" s="113"/>
-      <c r="F29" s="113"/>
+      <c r="B29" s="120"/>
+      <c r="C29" s="120"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="121"/>
+      <c r="F29" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2709,6 +2726,16 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2721,7 +2748,7 @@
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2967,7 +2994,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -3094,11 +3121,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="125" t="s">
@@ -3327,7 +3354,7 @@
   </sheetPr>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -3927,8 +3954,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3942,16 +3969,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
     </row>
     <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -4081,8 +4108,12 @@
       <c r="D8" s="57">
         <v>2</v>
       </c>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
+      <c r="E8" s="56">
+        <v>2</v>
+      </c>
+      <c r="F8" s="56">
+        <v>0</v>
+      </c>
       <c r="G8" s="58"/>
       <c r="H8" s="58">
         <v>45257</v>
@@ -4115,7 +4146,7 @@
       <c r="H10" s="56"/>
       <c r="I10" s="59"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
         <v>21</v>
       </c>
@@ -4132,13 +4163,17 @@
       <c r="F11" s="56">
         <v>0</v>
       </c>
-      <c r="G11" s="58"/>
+      <c r="G11" s="58">
+        <v>45205</v>
+      </c>
       <c r="H11" s="58">
         <v>45236</v>
       </c>
-      <c r="I11" s="59"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I11" s="59" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
         <v>22</v>
       </c>
@@ -4149,17 +4184,21 @@
       <c r="D12" s="57" t="s">
         <v>214</v>
       </c>
-      <c r="E12" s="56" t="s">
-        <v>214</v>
+      <c r="E12" s="56">
+        <v>5</v>
       </c>
       <c r="F12" s="56">
         <v>0</v>
       </c>
-      <c r="G12" s="58"/>
+      <c r="G12" s="58">
+        <v>45205</v>
+      </c>
       <c r="H12" s="58">
         <v>45236</v>
       </c>
-      <c r="I12" s="59"/>
+      <c r="I12" s="59" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
@@ -4178,13 +4217,17 @@
       <c r="F13" s="56">
         <v>0</v>
       </c>
-      <c r="G13" s="58"/>
+      <c r="G13" s="58">
+        <v>45205</v>
+      </c>
       <c r="H13" s="58">
         <v>45236</v>
       </c>
-      <c r="I13" s="59"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="59" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A14" s="28">
         <v>24</v>
       </c>
@@ -4201,11 +4244,15 @@
       <c r="F14" s="56">
         <v>0</v>
       </c>
-      <c r="G14" s="58"/>
+      <c r="G14" s="58">
+        <v>45243</v>
+      </c>
       <c r="H14" s="58">
         <v>45243</v>
       </c>
-      <c r="I14" s="59"/>
+      <c r="I14" s="59" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="28"/>
@@ -4250,11 +4297,15 @@
       <c r="F17" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="G17" s="58"/>
+      <c r="G17" s="58">
+        <v>45243</v>
+      </c>
       <c r="H17" s="58">
         <v>45243</v>
       </c>
-      <c r="I17" s="59"/>
+      <c r="I17" s="59" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
@@ -4268,16 +4319,20 @@
         <v>2</v>
       </c>
       <c r="E18" s="56">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F18" s="56">
-        <v>1</v>
-      </c>
-      <c r="G18" s="58"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="58">
+        <v>45243</v>
+      </c>
       <c r="H18" s="58">
         <v>45243</v>
       </c>
-      <c r="I18" s="59"/>
+      <c r="I18" s="59" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="28">
@@ -4288,19 +4343,23 @@
       </c>
       <c r="C19" s="56"/>
       <c r="D19" s="57">
+        <v>4</v>
+      </c>
+      <c r="E19" s="56">
+        <v>3</v>
+      </c>
+      <c r="F19" s="56">
         <v>1</v>
       </c>
-      <c r="E19" s="56">
-        <v>1</v>
-      </c>
-      <c r="F19" s="56">
-        <v>0</v>
-      </c>
-      <c r="G19" s="58"/>
+      <c r="G19" s="58">
+        <v>45250</v>
+      </c>
       <c r="H19" s="58">
         <v>45250</v>
       </c>
-      <c r="I19" s="59"/>
+      <c r="I19" s="59" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
@@ -4315,7 +4374,9 @@
       <c r="F20" s="56"/>
       <c r="G20" s="56"/>
       <c r="H20" s="56"/>
-      <c r="I20" s="59"/>
+      <c r="I20" s="66" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="28"/>
@@ -4354,17 +4415,21 @@
       <c r="D23" s="64">
         <v>1</v>
       </c>
-      <c r="E23" s="65" t="s">
-        <v>214</v>
-      </c>
-      <c r="F23" s="65" t="s">
-        <v>214</v>
-      </c>
-      <c r="G23" s="58"/>
+      <c r="E23" s="65">
+        <v>1</v>
+      </c>
+      <c r="F23" s="65">
+        <v>0</v>
+      </c>
+      <c r="G23" s="58">
+        <v>45250</v>
+      </c>
       <c r="H23" s="108">
         <v>45243</v>
       </c>
-      <c r="I23" s="66"/>
+      <c r="I23" s="66" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="63">
@@ -4379,7 +4444,9 @@
       <c r="F24" s="65"/>
       <c r="G24" s="58"/>
       <c r="H24" s="65"/>
-      <c r="I24" s="66"/>
+      <c r="I24" s="66" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="63">
@@ -4405,15 +4472,17 @@
       </c>
       <c r="C26" s="56"/>
       <c r="D26" s="64">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E26" s="65">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F26" s="65">
         <v>1</v>
       </c>
-      <c r="G26" s="58"/>
+      <c r="G26" s="58">
+        <v>45250</v>
+      </c>
       <c r="H26" s="108">
         <v>45250</v>
       </c>
@@ -4436,7 +4505,9 @@
       <c r="F27" s="65">
         <v>0</v>
       </c>
-      <c r="G27" s="58"/>
+      <c r="G27" s="108">
+        <v>45257</v>
+      </c>
       <c r="H27" s="108">
         <v>45257</v>
       </c>
@@ -4459,7 +4530,9 @@
       <c r="F28" s="65">
         <v>0</v>
       </c>
-      <c r="G28" s="58"/>
+      <c r="G28" s="108">
+        <v>45257</v>
+      </c>
       <c r="H28" s="108">
         <v>45257</v>
       </c>
@@ -4478,7 +4551,9 @@
       <c r="F29" s="56"/>
       <c r="G29" s="58"/>
       <c r="H29" s="56"/>
-      <c r="I29" s="59"/>
+      <c r="I29" s="66" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="28">
@@ -4493,7 +4568,9 @@
       <c r="F30" s="56"/>
       <c r="G30" s="58"/>
       <c r="H30" s="56"/>
-      <c r="I30" s="59"/>
+      <c r="I30" s="66" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="63"/>
@@ -4542,11 +4619,11 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D35" s="49">
         <f>SUM(D10:D34)</f>
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E35" s="49">
         <f>SUM(E10:E34)</f>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="F35" s="49">
         <f>SUM(F10:F34)</f>
@@ -4563,8 +4640,8 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6159,7 +6236,7 @@
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="A25:C25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6427,7 +6504,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AZE von 11.03.2024 aktualisiert
</commit_message>
<xml_diff>
--- a/Project_Car_01_Documentation.xlsx
+++ b/Project_Car_01_Documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\group-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293FD148-8AD8-4BC3-AA52-14E91C4D2989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FD4458-47F6-448D-88E1-92F3CE11EB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="256">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1210,6 +1210,12 @@
   </si>
   <si>
     <t>Programmcode optimiert</t>
+  </si>
+  <si>
+    <t>Messwerte in cm ausgeben (Distanz gemessen und in Excel umgerechnet)</t>
+  </si>
+  <si>
+    <t>Probelauf mit neuem Code (Sensorwerte in cm)</t>
   </si>
 </sst>
 </file>
@@ -1921,12 +1927,42 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1935,36 +1971,6 @@
     </xf>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2475,14 +2481,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -2531,10 +2537,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="111" t="s">
+      <c r="E7" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="111"/>
+      <c r="F7" s="116"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -2545,8 +2551,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2557,8 +2563,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="113"/>
-      <c r="F9" s="113"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
@@ -2569,8 +2575,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="114"/>
-      <c r="F10" s="114"/>
+      <c r="E10" s="124"/>
+      <c r="F10" s="124"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2581,8 +2587,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="17"/>
@@ -2603,49 +2609,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="116"/>
-      <c r="C15" s="116"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
-      <c r="F15" s="116"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="117"/>
-      <c r="C17" s="117"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="120"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="117"/>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
+      <c r="B18" s="120"/>
+      <c r="C18" s="120"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="122"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="122"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="114"/>
+      <c r="D19" s="114"/>
+      <c r="E19" s="114"/>
+      <c r="F19" s="114"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
@@ -2658,64 +2664,74 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="123" t="s">
+      <c r="A23" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
+      <c r="B23" s="115"/>
+      <c r="C23" s="115"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="115"/>
+      <c r="F23" s="115"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="111" t="s">
+      <c r="A26" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="111"/>
-      <c r="C26" s="111"/>
-      <c r="D26" s="111" t="s">
+      <c r="B26" s="116"/>
+      <c r="C26" s="116"/>
+      <c r="D26" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
+      <c r="E26" s="116"/>
+      <c r="F26" s="116"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="119" t="s">
+      <c r="A27" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="119"/>
-      <c r="C27" s="119"/>
-      <c r="D27" s="124"/>
-      <c r="E27" s="124"/>
-      <c r="F27" s="124"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="118" t="s">
+      <c r="A28" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="118"/>
-      <c r="C28" s="118"/>
-      <c r="D28" s="119" t="s">
+      <c r="B28" s="110"/>
+      <c r="C28" s="110"/>
+      <c r="D28" s="111" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="111"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="120" t="s">
+      <c r="A29" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="120"/>
-      <c r="C29" s="120"/>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="121"/>
+      <c r="B29" s="112"/>
+      <c r="C29" s="112"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="113"/>
+      <c r="F29" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2726,16 +2742,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2747,8 +2753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E282F0E-D68B-4ABC-BD94-0D22FA301A66}">
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2998,14 +3004,26 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="2"/>
+      <c r="A24" s="40">
+        <v>45362</v>
+      </c>
+      <c r="B24" s="41">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="2"/>
+      <c r="A25" s="40">
+        <v>45362</v>
+      </c>
+      <c r="B25" s="41">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="41"/>
@@ -3121,11 +3139,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="125" t="s">
@@ -3354,7 +3372,7 @@
   </sheetPr>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -3969,16 +3987,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="121" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
     </row>
     <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -6235,8 +6253,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6508,14 +6526,26 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="41"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="2"/>
+      <c r="A26" s="40">
+        <v>45362</v>
+      </c>
+      <c r="B26" s="41">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="41"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="2"/>
+      <c r="A27" s="40">
+        <v>45362</v>
+      </c>
+      <c r="B27" s="41">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="41"/>

</xml_diff>